<commit_message>
add: prediksi ternak API
</commit_message>
<xml_diff>
--- a/public/static/Data Produksi Susu.xlsx
+++ b/public/static/Data Produksi Susu.xlsx
@@ -43,7 +43,7 @@
     <t>Ternak ID 5</t>
   </si>
   <si>
-    <t>1/1/2021</t>
+    <t>7/6/2023</t>
   </si>
   <si>
     <t>-</t>
@@ -52,7 +52,7 @@
     <t>Perkawinan</t>
   </si>
   <si>
-    <t>Melahirkan</t>
+    <t>Laktasi</t>
   </si>
   <si>
     <t>Pemasukan</t>
@@ -86,7 +86,7 @@
       <b/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,7 +95,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF6a00"/>
+        <fgColor rgb="FF00f4FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -110,17 +110,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFb400"/>
+        <fgColor rgb="FF0090FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -130,12 +125,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8200"/>
+        <fgColor rgb="FF00c8FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF3800"/>
+        <fgColor rgb="FFFF8d00"/>
       </patternFill>
     </fill>
   </fills>
@@ -158,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -188,9 +183,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -591,7 +583,7 @@
         <v>1724</v>
       </c>
       <c r="E2" s="3">
-        <v>720</v>
+        <v>1800</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
@@ -608,7 +600,7 @@
       <c r="J2" s="4">
         <v>0</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="4">
@@ -620,7 +612,7 @@
       <c r="N2" s="4">
         <v>0</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -637,8 +629,8 @@
       <c r="D3" s="2">
         <v>1724</v>
       </c>
-      <c r="E3" s="8">
-        <v>1220</v>
+      <c r="E3" s="7">
+        <v>3050</v>
       </c>
       <c r="F3" s="4">
         <v>0</v>
@@ -646,7 +638,7 @@
       <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>2100</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -655,10 +647,10 @@
       <c r="J3" s="4">
         <v>0</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="8">
         <v>2100</v>
       </c>
       <c r="M3" s="6" t="s">
@@ -667,7 +659,7 @@
       <c r="N3" s="4">
         <v>0</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -684,8 +676,8 @@
       <c r="D4" s="2">
         <v>1724</v>
       </c>
-      <c r="E4" s="10">
-        <v>880</v>
+      <c r="E4" s="9">
+        <v>2200</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
@@ -693,7 +685,7 @@
       <c r="G4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>2200</v>
       </c>
       <c r="I4" s="6" t="s">
@@ -702,10 +694,10 @@
       <c r="J4" s="4">
         <v>0</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="8">
         <v>2200</v>
       </c>
       <c r="M4" s="6" t="s">
@@ -714,7 +706,7 @@
       <c r="N4" s="4">
         <v>0</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -731,8 +723,8 @@
       <c r="D5" s="2">
         <v>1724</v>
       </c>
-      <c r="E5" s="11">
-        <v>380</v>
+      <c r="E5" s="10">
+        <v>950</v>
       </c>
       <c r="F5" s="4">
         <v>0</v>
@@ -749,7 +741,7 @@
       <c r="J5" s="4">
         <v>0</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="4">
@@ -761,7 +753,7 @@
       <c r="N5" s="4">
         <v>0</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="6" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>